<commit_message>
fixed double counts in soy
</commit_message>
<xml_diff>
--- a/runs/acres22young/reports/soyCountACRES131.xlsx
+++ b/runs/acres22young/reports/soyCountACRES131.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="F1" s="10" t="inlineStr">
         <is>
-          <t>corn-n-soy-v1-exp</t>
+          <t>corn-n-soy-v2-exp</t>
         </is>
       </c>
       <c r="G1" s="10" t="inlineStr">
@@ -531,12 +531,12 @@
       </c>
       <c r="H1" s="10" t="inlineStr">
         <is>
-          <t>onlySoy-v1-exp</t>
+          <t>onlySoy-v2-exp</t>
         </is>
       </c>
       <c r="I1" s="10" t="inlineStr">
         <is>
-          <t>Diff: corn-n-soy-v1-exp</t>
+          <t>Diff: corn-n-soy-v2-exp</t>
         </is>
       </c>
       <c r="J1" s="10" t="inlineStr">
@@ -546,12 +546,12 @@
       </c>
       <c r="K1" s="10" t="inlineStr">
         <is>
-          <t>Diff: onlySoy-v1-exp</t>
+          <t>Diff: onlySoy-v2-exp</t>
         </is>
       </c>
       <c r="L1" s="10" t="inlineStr">
         <is>
-          <t>Error %: corn-n-soy-v1-exp</t>
+          <t>Error %: corn-n-soy-v2-exp</t>
         </is>
       </c>
       <c r="M1" s="10" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="N1" s="10" t="inlineStr">
         <is>
-          <t>Error %: onlySoy-v1-exp</t>
+          <t>Error %: onlySoy-v2-exp</t>
         </is>
       </c>
     </row>
@@ -584,31 +584,31 @@
         <v>214</v>
       </c>
       <c r="F2" t="n">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="G2" t="n">
         <v>1366</v>
       </c>
       <c r="H2" t="n">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="I2" t="n">
-        <v>-69</v>
+        <v>-92</v>
       </c>
       <c r="J2" t="n">
         <v>1152</v>
       </c>
       <c r="K2" t="n">
-        <v>-144</v>
+        <v>-132</v>
       </c>
       <c r="L2" t="n">
-        <v>-32.24299065420561</v>
+        <v>-42.99065420560748</v>
       </c>
       <c r="M2" t="n">
         <v>538.3177570093458</v>
       </c>
       <c r="N2" t="n">
-        <v>-67.28971962616822</v>
+        <v>-61.6822429906542</v>
       </c>
     </row>
     <row r="3">
@@ -630,31 +630,31 @@
         <v>117</v>
       </c>
       <c r="F3" t="n">
-        <v>193</v>
+        <v>93</v>
       </c>
       <c r="G3" t="n">
         <v>1028</v>
       </c>
       <c r="H3" t="n">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="I3" t="n">
-        <v>76</v>
+        <v>-24</v>
       </c>
       <c r="J3" t="n">
         <v>911</v>
       </c>
       <c r="K3" t="n">
-        <v>-19</v>
+        <v>-10</v>
       </c>
       <c r="L3" t="n">
-        <v>64.95726495726495</v>
+        <v>-20.51282051282051</v>
       </c>
       <c r="M3" t="n">
         <v>778.6324786324786</v>
       </c>
       <c r="N3" t="n">
-        <v>-16.23931623931624</v>
+        <v>-8.547008547008547</v>
       </c>
     </row>
     <row r="4">
@@ -674,31 +674,31 @@
         <v>106</v>
       </c>
       <c r="F4" t="n">
-        <v>256</v>
+        <v>156</v>
       </c>
       <c r="G4" t="n">
         <v>1933</v>
       </c>
       <c r="H4" t="n">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="I4" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="J4" t="n">
         <v>1827</v>
       </c>
       <c r="K4" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="L4" t="n">
-        <v>141.5094339622642</v>
+        <v>47.16981132075472</v>
       </c>
       <c r="M4" t="n">
         <v>1723.584905660377</v>
       </c>
       <c r="N4" t="n">
-        <v>5.660377358490567</v>
+        <v>20.75471698113208</v>
       </c>
     </row>
     <row r="5">
@@ -718,31 +718,31 @@
         <v>145</v>
       </c>
       <c r="F5" t="n">
-        <v>314</v>
+        <v>185</v>
       </c>
       <c r="G5" t="n">
         <v>1580</v>
       </c>
       <c r="H5" t="n">
-        <v>140</v>
+        <v>158</v>
       </c>
       <c r="I5" t="n">
-        <v>169</v>
+        <v>40</v>
       </c>
       <c r="J5" t="n">
         <v>1435</v>
       </c>
       <c r="K5" t="n">
-        <v>-5</v>
+        <v>13</v>
       </c>
       <c r="L5" t="n">
-        <v>116.551724137931</v>
+        <v>27.58620689655172</v>
       </c>
       <c r="M5" t="n">
         <v>989.655172413793</v>
       </c>
       <c r="N5" t="n">
-        <v>-3.448275862068965</v>
+        <v>8.96551724137931</v>
       </c>
     </row>
     <row r="6">
@@ -764,31 +764,31 @@
         <v>89</v>
       </c>
       <c r="F6" t="n">
-        <v>325</v>
+        <v>303</v>
       </c>
       <c r="G6" t="n">
         <v>1891</v>
       </c>
       <c r="H6" t="n">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="I6" t="n">
-        <v>236</v>
+        <v>214</v>
       </c>
       <c r="J6" t="n">
         <v>1802</v>
       </c>
       <c r="K6" t="n">
-        <v>199</v>
+        <v>213</v>
       </c>
       <c r="L6" t="n">
-        <v>265.1685393258427</v>
+        <v>240.4494382022472</v>
       </c>
       <c r="M6" t="n">
         <v>2024.719101123595</v>
       </c>
       <c r="N6" t="n">
-        <v>223.5955056179775</v>
+        <v>239.3258426966292</v>
       </c>
     </row>
     <row r="7">
@@ -810,31 +810,31 @@
         <v>97</v>
       </c>
       <c r="F7" t="n">
-        <v>447</v>
+        <v>206</v>
       </c>
       <c r="G7" t="n">
         <v>824</v>
       </c>
       <c r="H7" t="n">
-        <v>335</v>
+        <v>171</v>
       </c>
       <c r="I7" t="n">
-        <v>350</v>
+        <v>109</v>
       </c>
       <c r="J7" t="n">
         <v>727</v>
       </c>
       <c r="K7" t="n">
-        <v>238</v>
+        <v>74</v>
       </c>
       <c r="L7" t="n">
-        <v>360.8247422680412</v>
+        <v>112.3711340206186</v>
       </c>
       <c r="M7" t="n">
         <v>749.4845360824743</v>
       </c>
       <c r="N7" t="n">
-        <v>245.3608247422681</v>
+        <v>76.28865979381443</v>
       </c>
     </row>
     <row r="8">
@@ -854,31 +854,31 @@
         <v>91</v>
       </c>
       <c r="F8" t="n">
-        <v>379</v>
+        <v>197</v>
       </c>
       <c r="G8" t="n">
         <v>1195</v>
       </c>
       <c r="H8" t="n">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="I8" t="n">
-        <v>288</v>
+        <v>106</v>
       </c>
       <c r="J8" t="n">
         <v>1104</v>
       </c>
       <c r="K8" t="n">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="L8" t="n">
-        <v>316.4835164835165</v>
+        <v>116.4835164835165</v>
       </c>
       <c r="M8" t="n">
         <v>1213.186813186813</v>
       </c>
       <c r="N8" t="n">
-        <v>236.2637362637363</v>
+        <v>214.2857142857143</v>
       </c>
     </row>
     <row r="9">
@@ -898,31 +898,31 @@
         <v>91</v>
       </c>
       <c r="F9" t="n">
-        <v>497</v>
+        <v>290</v>
       </c>
       <c r="G9" t="n">
         <v>1301</v>
       </c>
       <c r="H9" t="n">
-        <v>408</v>
+        <v>255</v>
       </c>
       <c r="I9" t="n">
-        <v>406</v>
+        <v>199</v>
       </c>
       <c r="J9" t="n">
         <v>1210</v>
       </c>
       <c r="K9" t="n">
-        <v>317</v>
+        <v>164</v>
       </c>
       <c r="L9" t="n">
-        <v>446.1538461538462</v>
+        <v>218.6813186813187</v>
       </c>
       <c r="M9" t="n">
         <v>1329.67032967033</v>
       </c>
       <c r="N9" t="n">
-        <v>348.3516483516484</v>
+        <v>180.2197802197802</v>
       </c>
     </row>
     <row r="10">
@@ -944,31 +944,31 @@
         <v>72</v>
       </c>
       <c r="F10" t="n">
-        <v>457</v>
+        <v>241</v>
       </c>
       <c r="G10" t="n">
         <v>1287</v>
       </c>
       <c r="H10" t="n">
-        <v>387</v>
+        <v>237</v>
       </c>
       <c r="I10" t="n">
-        <v>385</v>
+        <v>169</v>
       </c>
       <c r="J10" t="n">
         <v>1215</v>
       </c>
       <c r="K10" t="n">
-        <v>315</v>
+        <v>165</v>
       </c>
       <c r="L10" t="n">
-        <v>534.7222222222223</v>
+        <v>234.7222222222222</v>
       </c>
       <c r="M10" t="n">
         <v>1687.5</v>
       </c>
       <c r="N10" t="n">
-        <v>437.5</v>
+        <v>229.1666666666667</v>
       </c>
     </row>
     <row r="11">
@@ -990,31 +990,31 @@
         <v>91</v>
       </c>
       <c r="F11" t="n">
-        <v>395</v>
+        <v>231</v>
       </c>
       <c r="G11" t="n">
         <v>1195</v>
       </c>
       <c r="H11" t="n">
-        <v>321</v>
+        <v>226</v>
       </c>
       <c r="I11" t="n">
-        <v>304</v>
+        <v>140</v>
       </c>
       <c r="J11" t="n">
         <v>1104</v>
       </c>
       <c r="K11" t="n">
-        <v>230</v>
+        <v>135</v>
       </c>
       <c r="L11" t="n">
-        <v>334.0659340659341</v>
+        <v>153.8461538461539</v>
       </c>
       <c r="M11" t="n">
         <v>1213.186813186813</v>
       </c>
       <c r="N11" t="n">
-        <v>252.7472527472527</v>
+        <v>148.3516483516484</v>
       </c>
     </row>
     <row r="12">
@@ -1036,31 +1036,31 @@
         <v>126</v>
       </c>
       <c r="F12" t="n">
-        <v>413</v>
+        <v>153</v>
       </c>
       <c r="G12" t="n">
         <v>1651</v>
       </c>
       <c r="H12" t="n">
-        <v>324</v>
+        <v>145</v>
       </c>
       <c r="I12" t="n">
-        <v>287</v>
+        <v>27</v>
       </c>
       <c r="J12" t="n">
         <v>1525</v>
       </c>
       <c r="K12" t="n">
-        <v>198</v>
+        <v>19</v>
       </c>
       <c r="L12" t="n">
-        <v>227.7777777777778</v>
+        <v>21.42857142857143</v>
       </c>
       <c r="M12" t="n">
         <v>1210.31746031746</v>
       </c>
       <c r="N12" t="n">
-        <v>157.1428571428571</v>
+        <v>15.07936507936508</v>
       </c>
     </row>
     <row r="13">
@@ -1082,31 +1082,31 @@
         <v>75</v>
       </c>
       <c r="F13" t="n">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="G13" t="n">
         <v>1895</v>
       </c>
       <c r="H13" t="n">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="I13" t="n">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="J13" t="n">
         <v>1820</v>
       </c>
       <c r="K13" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="L13" t="n">
-        <v>92</v>
+        <v>57.33333333333334</v>
       </c>
       <c r="M13" t="n">
         <v>2426.666666666667</v>
       </c>
       <c r="N13" t="n">
-        <v>61.33333333333333</v>
+        <v>25.33333333333334</v>
       </c>
     </row>
     <row r="14">
@@ -1128,31 +1128,31 @@
         <v>166</v>
       </c>
       <c r="F14" t="n">
-        <v>240</v>
+        <v>128</v>
       </c>
       <c r="G14" t="n">
         <v>799</v>
       </c>
       <c r="H14" t="n">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I14" t="n">
-        <v>74</v>
+        <v>-38</v>
       </c>
       <c r="J14" t="n">
         <v>633</v>
       </c>
       <c r="K14" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L14" t="n">
-        <v>44.57831325301205</v>
+        <v>-22.89156626506024</v>
       </c>
       <c r="M14" t="n">
         <v>381.3253012048193</v>
       </c>
       <c r="N14" t="n">
-        <v>25.90361445783132</v>
+        <v>24.69879518072289</v>
       </c>
     </row>
     <row r="15">
@@ -1174,31 +1174,31 @@
         <v>760</v>
       </c>
       <c r="F15" t="n">
-        <v>840</v>
+        <v>516</v>
       </c>
       <c r="G15" t="n">
         <v>2100</v>
       </c>
       <c r="H15" t="n">
-        <v>599</v>
+        <v>502</v>
       </c>
       <c r="I15" t="n">
-        <v>80</v>
+        <v>-244</v>
       </c>
       <c r="J15" t="n">
         <v>1340</v>
       </c>
       <c r="K15" t="n">
-        <v>-161</v>
+        <v>-258</v>
       </c>
       <c r="L15" t="n">
-        <v>10.52631578947368</v>
+        <v>-32.10526315789474</v>
       </c>
       <c r="M15" t="n">
         <v>176.3157894736842</v>
       </c>
       <c r="N15" t="n">
-        <v>-21.18421052631579</v>
+        <v>-33.94736842105263</v>
       </c>
     </row>
     <row r="16">
@@ -1218,31 +1218,31 @@
         <v>133</v>
       </c>
       <c r="F16" t="n">
-        <v>405</v>
+        <v>309</v>
       </c>
       <c r="G16" t="n">
         <v>1870</v>
       </c>
       <c r="H16" t="n">
-        <v>244</v>
+        <v>193</v>
       </c>
       <c r="I16" t="n">
-        <v>272</v>
+        <v>176</v>
       </c>
       <c r="J16" t="n">
         <v>1737</v>
       </c>
       <c r="K16" t="n">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="L16" t="n">
-        <v>204.5112781954887</v>
+        <v>132.3308270676692</v>
       </c>
       <c r="M16" t="n">
         <v>1306.015037593985</v>
       </c>
       <c r="N16" t="n">
-        <v>83.45864661654136</v>
+        <v>45.11278195488722</v>
       </c>
     </row>
     <row r="17">
@@ -1264,31 +1264,31 @@
         <v>320</v>
       </c>
       <c r="F17" t="n">
-        <v>225</v>
+        <v>134</v>
       </c>
       <c r="G17" t="n">
         <v>673</v>
       </c>
       <c r="H17" t="n">
-        <v>144</v>
+        <v>71</v>
       </c>
       <c r="I17" t="n">
-        <v>-95</v>
+        <v>-186</v>
       </c>
       <c r="J17" t="n">
         <v>353</v>
       </c>
       <c r="K17" t="n">
-        <v>-176</v>
+        <v>-249</v>
       </c>
       <c r="L17" t="n">
-        <v>-29.6875</v>
+        <v>-58.12500000000001</v>
       </c>
       <c r="M17" t="n">
         <v>110.3125</v>
       </c>
       <c r="N17" t="n">
-        <v>-55.00000000000001</v>
+        <v>-77.8125</v>
       </c>
     </row>
     <row r="18">
@@ -1310,31 +1310,31 @@
         <v>720</v>
       </c>
       <c r="F18" t="n">
-        <v>992</v>
+        <v>552</v>
       </c>
       <c r="G18" t="n">
         <v>1541</v>
       </c>
       <c r="H18" t="n">
-        <v>790</v>
+        <v>498</v>
       </c>
       <c r="I18" t="n">
-        <v>272</v>
+        <v>-168</v>
       </c>
       <c r="J18" t="n">
         <v>821</v>
       </c>
       <c r="K18" t="n">
-        <v>70</v>
+        <v>-222</v>
       </c>
       <c r="L18" t="n">
-        <v>37.77777777777778</v>
+        <v>-23.33333333333333</v>
       </c>
       <c r="M18" t="n">
         <v>114.0277777777778</v>
       </c>
       <c r="N18" t="n">
-        <v>9.722222222222223</v>
+        <v>-30.83333333333334</v>
       </c>
     </row>
     <row r="19">
@@ -1356,31 +1356,31 @@
         <v>634</v>
       </c>
       <c r="F19" t="n">
-        <v>430</v>
+        <v>344</v>
       </c>
       <c r="G19" t="n">
         <v>1513</v>
       </c>
       <c r="H19" t="n">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="I19" t="n">
-        <v>-204</v>
+        <v>-290</v>
       </c>
       <c r="J19" t="n">
         <v>879</v>
       </c>
       <c r="K19" t="n">
-        <v>-333</v>
+        <v>-340</v>
       </c>
       <c r="L19" t="n">
-        <v>-32.17665615141956</v>
+        <v>-45.74132492113564</v>
       </c>
       <c r="M19" t="n">
         <v>138.6435331230284</v>
       </c>
       <c r="N19" t="n">
-        <v>-52.52365930599369</v>
+        <v>-53.62776025236593</v>
       </c>
     </row>
     <row r="20">
@@ -1400,31 +1400,31 @@
         <v>294</v>
       </c>
       <c r="F20" t="n">
-        <v>257</v>
+        <v>117</v>
       </c>
       <c r="G20" t="n">
         <v>1357</v>
       </c>
       <c r="H20" t="n">
-        <v>152</v>
+        <v>113</v>
       </c>
       <c r="I20" t="n">
-        <v>-37</v>
+        <v>-177</v>
       </c>
       <c r="J20" t="n">
         <v>1063</v>
       </c>
       <c r="K20" t="n">
-        <v>-142</v>
+        <v>-181</v>
       </c>
       <c r="L20" t="n">
-        <v>-12.58503401360544</v>
+        <v>-60.20408163265306</v>
       </c>
       <c r="M20" t="n">
         <v>361.5646258503401</v>
       </c>
       <c r="N20" t="n">
-        <v>-48.29931972789115</v>
+        <v>-61.56462585034014</v>
       </c>
     </row>
     <row r="21">
@@ -1446,31 +1446,31 @@
         <v>426</v>
       </c>
       <c r="F21" t="n">
-        <v>599</v>
+        <v>368</v>
       </c>
       <c r="G21" t="n">
         <v>1000</v>
       </c>
       <c r="H21" t="n">
-        <v>374</v>
+        <v>231</v>
       </c>
       <c r="I21" t="n">
-        <v>173</v>
+        <v>-58</v>
       </c>
       <c r="J21" t="n">
         <v>574</v>
       </c>
       <c r="K21" t="n">
-        <v>-52</v>
+        <v>-195</v>
       </c>
       <c r="L21" t="n">
-        <v>40.61032863849765</v>
+        <v>-13.6150234741784</v>
       </c>
       <c r="M21" t="n">
         <v>134.7417840375587</v>
       </c>
       <c r="N21" t="n">
-        <v>-12.20657276995305</v>
+        <v>-45.77464788732394</v>
       </c>
     </row>
     <row r="22">
@@ -1492,31 +1492,31 @@
         <v>357</v>
       </c>
       <c r="F22" t="n">
-        <v>258</v>
+        <v>153</v>
       </c>
       <c r="G22" t="n">
         <v>1292</v>
       </c>
       <c r="H22" t="n">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="I22" t="n">
-        <v>-99</v>
+        <v>-204</v>
       </c>
       <c r="J22" t="n">
         <v>935</v>
       </c>
       <c r="K22" t="n">
-        <v>-169</v>
+        <v>-161</v>
       </c>
       <c r="L22" t="n">
-        <v>-27.73109243697479</v>
+        <v>-57.14285714285714</v>
       </c>
       <c r="M22" t="n">
         <v>261.9047619047619</v>
       </c>
       <c r="N22" t="n">
-        <v>-47.33893557422969</v>
+        <v>-45.09803921568628</v>
       </c>
     </row>
     <row r="23">
@@ -1538,31 +1538,31 @@
         <v>355</v>
       </c>
       <c r="F23" t="n">
-        <v>306</v>
+        <v>259</v>
       </c>
       <c r="G23" t="n">
         <v>1615</v>
       </c>
       <c r="H23" t="n">
-        <v>249</v>
+        <v>280</v>
       </c>
       <c r="I23" t="n">
-        <v>-49</v>
+        <v>-96</v>
       </c>
       <c r="J23" t="n">
         <v>1260</v>
       </c>
       <c r="K23" t="n">
-        <v>-106</v>
+        <v>-75</v>
       </c>
       <c r="L23" t="n">
-        <v>-13.80281690140845</v>
+        <v>-27.04225352112676</v>
       </c>
       <c r="M23" t="n">
         <v>354.9295774647887</v>
       </c>
       <c r="N23" t="n">
-        <v>-29.85915492957746</v>
+        <v>-21.12676056338028</v>
       </c>
     </row>
     <row r="24">
@@ -1582,31 +1582,31 @@
         <v>718</v>
       </c>
       <c r="F24" t="n">
-        <v>1056</v>
+        <v>809</v>
       </c>
       <c r="G24" t="n">
         <v>2000</v>
       </c>
       <c r="H24" t="n">
-        <v>824</v>
+        <v>642</v>
       </c>
       <c r="I24" t="n">
-        <v>338</v>
+        <v>91</v>
       </c>
       <c r="J24" t="n">
         <v>1282</v>
       </c>
       <c r="K24" t="n">
-        <v>106</v>
+        <v>-76</v>
       </c>
       <c r="L24" t="n">
-        <v>47.07520891364902</v>
+        <v>12.67409470752089</v>
       </c>
       <c r="M24" t="n">
         <v>178.5515320334262</v>
       </c>
       <c r="N24" t="n">
-        <v>14.76323119777159</v>
+        <v>-10.5849582172702</v>
       </c>
     </row>
     <row r="25">
@@ -1626,31 +1626,31 @@
         <v>613</v>
       </c>
       <c r="F25" t="n">
-        <v>672</v>
+        <v>466</v>
       </c>
       <c r="G25" t="n">
         <v>1621</v>
       </c>
       <c r="H25" t="n">
-        <v>525</v>
+        <v>437</v>
       </c>
       <c r="I25" t="n">
-        <v>59</v>
+        <v>-147</v>
       </c>
       <c r="J25" t="n">
         <v>1008</v>
       </c>
       <c r="K25" t="n">
-        <v>-88</v>
+        <v>-176</v>
       </c>
       <c r="L25" t="n">
-        <v>9.624796084828711</v>
+        <v>-23.98042414355628</v>
       </c>
       <c r="M25" t="n">
         <v>164.4371941272431</v>
       </c>
       <c r="N25" t="n">
-        <v>-14.35562805872757</v>
+        <v>-28.71125611745514</v>
       </c>
     </row>
     <row r="26">
@@ -1672,31 +1672,31 @@
         <v>894</v>
       </c>
       <c r="F26" t="n">
-        <v>2178</v>
+        <v>1918</v>
       </c>
       <c r="G26" t="n">
         <v>4543</v>
       </c>
       <c r="H26" t="n">
-        <v>2018</v>
+        <v>1880</v>
       </c>
       <c r="I26" t="n">
-        <v>1284</v>
+        <v>1024</v>
       </c>
       <c r="J26" t="n">
         <v>3649</v>
       </c>
       <c r="K26" t="n">
-        <v>1124</v>
+        <v>986</v>
       </c>
       <c r="L26" t="n">
-        <v>143.6241610738255</v>
+        <v>114.5413870246085</v>
       </c>
       <c r="M26" t="n">
         <v>408.165548098434</v>
       </c>
       <c r="N26" t="n">
-        <v>125.7270693512304</v>
+        <v>110.2908277404922</v>
       </c>
     </row>
     <row r="27">
@@ -1718,31 +1718,31 @@
         <v>29</v>
       </c>
       <c r="F27" t="n">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="G27" t="n">
         <v>2091</v>
       </c>
       <c r="H27" t="n">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="I27" t="n">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="J27" t="n">
         <v>2062</v>
       </c>
       <c r="K27" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="L27" t="n">
-        <v>255.1724137931035</v>
+        <v>196.551724137931</v>
       </c>
       <c r="M27" t="n">
         <v>7110.344827586207</v>
       </c>
       <c r="N27" t="n">
-        <v>227.5862068965517</v>
+        <v>237.9310344827586</v>
       </c>
     </row>
     <row r="28">
@@ -1762,31 +1762,31 @@
         <v>74</v>
       </c>
       <c r="F28" t="n">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="G28" t="n">
         <v>1270</v>
       </c>
       <c r="H28" t="n">
-        <v>133</v>
+        <v>179</v>
       </c>
       <c r="I28" t="n">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="J28" t="n">
         <v>1196</v>
       </c>
       <c r="K28" t="n">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="L28" t="n">
-        <v>159.4594594594595</v>
+        <v>114.8648648648649</v>
       </c>
       <c r="M28" t="n">
         <v>1616.216216216216</v>
       </c>
       <c r="N28" t="n">
-        <v>79.72972972972973</v>
+        <v>141.8918918918919</v>
       </c>
     </row>
     <row r="29">
@@ -1806,31 +1806,31 @@
         <v>296</v>
       </c>
       <c r="F29" t="n">
-        <v>603</v>
+        <v>559</v>
       </c>
       <c r="G29" t="n">
         <v>1257</v>
       </c>
       <c r="H29" t="n">
-        <v>467</v>
+        <v>353</v>
       </c>
       <c r="I29" t="n">
-        <v>307</v>
+        <v>263</v>
       </c>
       <c r="J29" t="n">
         <v>961</v>
       </c>
       <c r="K29" t="n">
-        <v>171</v>
+        <v>57</v>
       </c>
       <c r="L29" t="n">
-        <v>103.7162162162162</v>
+        <v>88.85135135135135</v>
       </c>
       <c r="M29" t="n">
         <v>324.6621621621621</v>
       </c>
       <c r="N29" t="n">
-        <v>57.77027027027027</v>
+        <v>19.25675675675676</v>
       </c>
     </row>
     <row r="30">
@@ -1852,31 +1852,31 @@
         <v>497</v>
       </c>
       <c r="F30" t="n">
-        <v>633</v>
+        <v>595</v>
       </c>
       <c r="G30" t="n">
         <v>3076</v>
       </c>
       <c r="H30" t="n">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="I30" t="n">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="J30" t="n">
         <v>2579</v>
       </c>
       <c r="K30" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L30" t="n">
-        <v>27.36418511066399</v>
+        <v>19.71830985915493</v>
       </c>
       <c r="M30" t="n">
         <v>518.9134808853119</v>
       </c>
       <c r="N30" t="n">
-        <v>17.10261569416499</v>
+        <v>17.30382293762575</v>
       </c>
     </row>
     <row r="31">
@@ -1898,31 +1898,31 @@
         <v>324</v>
       </c>
       <c r="F31" t="n">
-        <v>440</v>
+        <v>326</v>
       </c>
       <c r="G31" t="n">
         <v>1205</v>
       </c>
       <c r="H31" t="n">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="I31" t="n">
-        <v>116</v>
+        <v>2</v>
       </c>
       <c r="J31" t="n">
         <v>881</v>
       </c>
       <c r="K31" t="n">
-        <v>-55</v>
+        <v>-45</v>
       </c>
       <c r="L31" t="n">
-        <v>35.80246913580247</v>
+        <v>0.6172839506172839</v>
       </c>
       <c r="M31" t="n">
         <v>271.9135802469136</v>
       </c>
       <c r="N31" t="n">
-        <v>-16.97530864197531</v>
+        <v>-13.88888888888889</v>
       </c>
     </row>
     <row r="32">
@@ -1944,31 +1944,31 @@
         <v>77</v>
       </c>
       <c r="F32" t="n">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="G32" t="n">
         <v>1378</v>
       </c>
       <c r="H32" t="n">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="I32" t="n">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="J32" t="n">
         <v>1301</v>
       </c>
       <c r="K32" t="n">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="L32" t="n">
-        <v>146.7532467532467</v>
+        <v>89.6103896103896</v>
       </c>
       <c r="M32" t="n">
         <v>1689.61038961039</v>
       </c>
       <c r="N32" t="n">
-        <v>71.42857142857143</v>
+        <v>106.4935064935065</v>
       </c>
     </row>
     <row r="33">
@@ -1988,31 +1988,31 @@
         <v>187</v>
       </c>
       <c r="F33" t="n">
-        <v>402</v>
+        <v>366</v>
       </c>
       <c r="G33" t="n">
         <v>2914</v>
       </c>
       <c r="H33" t="n">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="I33" t="n">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="J33" t="n">
         <v>2727</v>
       </c>
       <c r="K33" t="n">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="L33" t="n">
-        <v>114.9732620320856</v>
+        <v>95.72192513368985</v>
       </c>
       <c r="M33" t="n">
         <v>1458.288770053476</v>
       </c>
       <c r="N33" t="n">
-        <v>100.5347593582888</v>
+        <v>93.58288770053476</v>
       </c>
     </row>
     <row r="34">
@@ -2034,31 +2034,31 @@
         <v>624</v>
       </c>
       <c r="F34" t="n">
-        <v>945</v>
+        <v>898</v>
       </c>
       <c r="G34" t="n">
         <v>2860</v>
       </c>
       <c r="H34" t="n">
-        <v>871</v>
+        <v>876</v>
       </c>
       <c r="I34" t="n">
-        <v>321</v>
+        <v>274</v>
       </c>
       <c r="J34" t="n">
         <v>2236</v>
       </c>
       <c r="K34" t="n">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="L34" t="n">
-        <v>51.44230769230769</v>
+        <v>43.91025641025641</v>
       </c>
       <c r="M34" t="n">
         <v>358.3333333333334</v>
       </c>
       <c r="N34" t="n">
-        <v>39.58333333333333</v>
+        <v>40.38461538461539</v>
       </c>
     </row>
     <row r="35">
@@ -2080,31 +2080,31 @@
         <v>565</v>
       </c>
       <c r="F35" t="n">
-        <v>1238</v>
+        <v>1206</v>
       </c>
       <c r="G35" t="n">
         <v>3217</v>
       </c>
       <c r="H35" t="n">
-        <v>1152</v>
+        <v>1208</v>
       </c>
       <c r="I35" t="n">
-        <v>673</v>
+        <v>641</v>
       </c>
       <c r="J35" t="n">
         <v>2652</v>
       </c>
       <c r="K35" t="n">
-        <v>587</v>
+        <v>643</v>
       </c>
       <c r="L35" t="n">
-        <v>119.1150442477876</v>
+        <v>113.4513274336283</v>
       </c>
       <c r="M35" t="n">
         <v>469.3805309734513</v>
       </c>
       <c r="N35" t="n">
-        <v>103.8938053097345</v>
+        <v>113.8053097345133</v>
       </c>
     </row>
     <row r="36">
@@ -2126,31 +2126,31 @@
         <v>115</v>
       </c>
       <c r="F36" t="n">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="G36" t="n">
         <v>2187</v>
       </c>
       <c r="H36" t="n">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="I36" t="n">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="J36" t="n">
         <v>2072</v>
       </c>
       <c r="K36" t="n">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="L36" t="n">
-        <v>227.8260869565217</v>
+        <v>216.5217391304348</v>
       </c>
       <c r="M36" t="n">
         <v>1801.739130434783</v>
       </c>
       <c r="N36" t="n">
-        <v>224.3478260869565</v>
+        <v>217.3913043478261</v>
       </c>
     </row>
     <row r="37">
@@ -2170,31 +2170,31 @@
         <v>207</v>
       </c>
       <c r="F37" t="n">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="G37" t="n">
         <v>2551</v>
       </c>
       <c r="H37" t="n">
-        <v>503</v>
+        <v>517</v>
       </c>
       <c r="I37" t="n">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="J37" t="n">
         <v>2344</v>
       </c>
       <c r="K37" t="n">
-        <v>296</v>
+        <v>310</v>
       </c>
       <c r="L37" t="n">
-        <v>150.7246376811594</v>
+        <v>148.3091787439614</v>
       </c>
       <c r="M37" t="n">
         <v>1132.367149758454</v>
       </c>
       <c r="N37" t="n">
-        <v>142.9951690821256</v>
+        <v>149.7584541062802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>